<commit_message>
Continue reading polidorou thesis
</commit_message>
<xml_diff>
--- a/PriliminaryDesign/Specifications.xlsx
+++ b/PriliminaryDesign/Specifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BipedProject\PriliminaryDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082738C6-E8B7-4268-A55E-B5AA9629586A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBF2222-FA48-4E27-ABA0-1E273D52D082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Comments</t>
   </si>
@@ -36,14 +36,27 @@
     <t>Specifications</t>
   </si>
   <si>
-    <t>Robot designs</t>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Actuators</t>
+  </si>
+  <si>
+    <t>1) High torque density
+2) Force transparency
+3) Mechanical robustness
+4) Energy efficieny
+5) Low mechanical impendance</t>
+  </si>
+  <si>
+    <t>PetrosPolidorouDiplomaThesisMotorDesign.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +71,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -87,11 +108,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -99,9 +121,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,15 +410,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -408,8 +435,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="130.19999999999999" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="../Bibliography/TotalBibliography/PetrosPolidorouDiplomaThesisMotorDesign.pdf" xr:uid="{D6FA8BB5-B337-47E3-BE06-96B1BCD89EAA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>